<commit_message>
v2.2: Adicionada integração com Telegram + melhorias de estrutura
</commit_message>
<xml_diff>
--- a/Relatorio_Jogos_0x0.xlsx
+++ b/Relatorio_Jogos_0x0.xlsx
@@ -514,12 +514,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Major League Soccer</t>
+          <t>Liga de Fútbol de Primera División</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Sporting KC</t>
+          <t>CS Herediano</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -527,7 +527,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>St. Louis City</t>
+          <t>CS Cartagines</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
@@ -535,11 +535,11 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>51'</t>
+          <t>43'</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
@@ -553,19 +553,19 @@
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>22:50:06</t>
+          <t>23:46:01</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Major League Soccer</t>
+          <t>USL Championship</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Houston Dynamo</t>
+          <t>Sacramento Republic FC</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -573,7 +573,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>LAFC</t>
+          <t>Louisville City FC</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
@@ -581,11 +581,11 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>40'</t>
+          <t>35'</t>
         </is>
       </c>
       <c r="G3" s="2" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
@@ -599,7 +599,7 @@
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>22:50:06</t>
+          <t>23:46:01</t>
         </is>
       </c>
     </row>
@@ -627,11 +627,11 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>42'</t>
+          <t>80'</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
@@ -645,7 +645,7 @@
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>22:50:06</t>
+          <t>23:46:02</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajuste na lógica de analise 0x0 e tempo entre 20 e 40min
</commit_message>
<xml_diff>
--- a/Relatorio_Jogos_0x0.xlsx
+++ b/Relatorio_Jogos_0x0.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Jogos 0x0" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Jogos 0x0'!$A$1:$J$4</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Jogos 0x0'!$A$1:$J$8</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -514,12 +514,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Liga de Fútbol de Primera División</t>
+          <t>Bundesliga</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>CS Herediano</t>
+          <t>St. Pauli</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -527,7 +527,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>CS Cartagines</t>
+          <t>Borussia Mönchengladbach</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
@@ -535,11 +535,11 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>43'</t>
+          <t>27'</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
@@ -548,24 +548,24 @@
       </c>
       <c r="I2" s="2" t="inlineStr">
         <is>
-          <t>05/04/2025</t>
+          <t>06/04/2025</t>
         </is>
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>23:46:01</t>
+          <t>10:57:25</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>USL Championship</t>
+          <t>Chance liga</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>Sacramento Republic FC</t>
+          <t>FK Mlada Boleslav</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -573,7 +573,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>Louisville City FC</t>
+          <t>FK Dukla Praga</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
@@ -581,11 +581,11 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>35'</t>
+          <t>25'</t>
         </is>
       </c>
       <c r="G3" s="2" t="n">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
@@ -594,24 +594,24 @@
       </c>
       <c r="I3" s="2" t="inlineStr">
         <is>
-          <t>05/04/2025</t>
+          <t>06/04/2025</t>
         </is>
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>23:46:01</t>
+          <t>10:57:26</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>USL League One</t>
+          <t>Liga Pro</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Spokane Velocity</t>
+          <t>Kheybar</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -619,7 +619,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Hearts of Pine</t>
+          <t>Shams Azar</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
@@ -627,11 +627,11 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>80'</t>
+          <t>25'</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
@@ -640,17 +640,201 @@
       </c>
       <c r="I4" s="2" t="inlineStr">
         <is>
-          <t>05/04/2025</t>
+          <t>06/04/2025</t>
         </is>
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>23:46:02</t>
+          <t>10:57:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Niké Liga</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>MFK Ruzomberok</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>MFK Dukla Banska Bystrica</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>25'</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="H5" s="2" t="inlineStr">
+        <is>
+          <t>Em Andamento</t>
+        </is>
+      </c>
+      <c r="I5" s="2" t="inlineStr">
+        <is>
+          <t>06/04/2025</t>
+        </is>
+      </c>
+      <c r="J5" s="2" t="inlineStr">
+        <is>
+          <t>10:57:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Niké Liga</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>FK Kosice</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>FC Spartak Trnava</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>20'</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="n">
+        <v>20</v>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>Em Andamento</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="inlineStr">
+        <is>
+          <t>06/04/2025</t>
+        </is>
+      </c>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>10:57:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Russian Premier League</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>Rostov</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>Spartak Moscovo</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>25'</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>Em Andamento</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>06/04/2025</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>10:57:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Scottish Premiership</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>Heart of Midlothian FC</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>Dundee United</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>25'</t>
+        </is>
+      </c>
+      <c r="G8" s="2" t="n">
+        <v>25</v>
+      </c>
+      <c r="H8" s="2" t="inlineStr">
+        <is>
+          <t>Em Andamento</t>
+        </is>
+      </c>
+      <c r="I8" s="2" t="inlineStr">
+        <is>
+          <t>06/04/2025</t>
+        </is>
+      </c>
+      <c r="J8" s="2" t="inlineStr">
+        <is>
+          <t>10:57:30</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J4"/>
+  <autoFilter ref="A1:J8"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
implementação de loop para monitoramente a cada 15 minutos
</commit_message>
<xml_diff>
--- a/Relatorio_Jogos_0x0.xlsx
+++ b/Relatorio_Jogos_0x0.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Jogos 0x0" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Jogos 0x0'!$A$1:$J$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Jogos 0x0'!$A$1:$J$6</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -514,12 +514,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Bundesliga</t>
+          <t>Campeonato Islandês</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>St. Pauli</t>
+          <t>Valur Reykjavik</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -527,7 +527,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>Borussia Mönchengladbach</t>
+          <t>IF Vestri</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
@@ -535,11 +535,11 @@
       </c>
       <c r="F2" s="2" t="inlineStr">
         <is>
-          <t>27'</t>
+          <t>40'</t>
         </is>
       </c>
       <c r="G2" s="2" t="n">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="H2" s="2" t="inlineStr">
         <is>
@@ -553,19 +553,19 @@
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>10:57:25</t>
+          <t>11:42:30</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Chance liga</t>
+          <t>Liga Nacional de Futebol</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>FK Mlada Boleslav</t>
+          <t>Torpedo Moscovo</t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
@@ -573,7 +573,7 @@
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>FK Dukla Praga</t>
+          <t>SK Rotor Volgograd</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
@@ -581,11 +581,11 @@
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>25'</t>
+          <t>40'</t>
         </is>
       </c>
       <c r="G3" s="2" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H3" s="2" t="inlineStr">
         <is>
@@ -599,19 +599,19 @@
       </c>
       <c r="J3" s="2" t="inlineStr">
         <is>
-          <t>10:57:26</t>
+          <t>11:42:31</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Liga Pro</t>
+          <t>Liga Principal</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>Kheybar</t>
+          <t>FC Gomel</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
@@ -619,7 +619,7 @@
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Shams Azar</t>
+          <t>FC Slavia Mozyr</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
@@ -627,11 +627,11 @@
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>25'</t>
+          <t>40'</t>
         </is>
       </c>
       <c r="G4" s="2" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="H4" s="2" t="inlineStr">
         <is>
@@ -645,19 +645,19 @@
       </c>
       <c r="J4" s="2" t="inlineStr">
         <is>
-          <t>10:57:26</t>
+          <t>11:42:32</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Niké Liga</t>
+          <t>Primeira Liga de Futebol Profissional</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>MFK Ruzomberok</t>
+          <t>Beroe Stara Zagora</t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
@@ -665,7 +665,7 @@
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>MFK Dukla Banska Bystrica</t>
+          <t>Levski Sófia</t>
         </is>
       </c>
       <c r="E5" s="2" t="n">
@@ -673,11 +673,11 @@
       </c>
       <c r="F5" s="2" t="inlineStr">
         <is>
-          <t>25'</t>
+          <t>24'</t>
         </is>
       </c>
       <c r="G5" s="2" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="2" t="inlineStr">
         <is>
@@ -691,19 +691,19 @@
       </c>
       <c r="J5" s="2" t="inlineStr">
         <is>
-          <t>10:57:27</t>
+          <t>11:42:33</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Niké Liga</t>
+          <t>Torneo Federal A</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>FK Kosice</t>
+          <t>CD Santamarina Tandil</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
@@ -711,7 +711,7 @@
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>FC Spartak Trnava</t>
+          <t>Deportivo Rincón</t>
         </is>
       </c>
       <c r="E6" s="2" t="n">
@@ -719,11 +719,11 @@
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>20'</t>
+          <t>36'</t>
         </is>
       </c>
       <c r="G6" s="2" t="n">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="H6" s="2" t="inlineStr">
         <is>
@@ -737,104 +737,12 @@
       </c>
       <c r="J6" s="2" t="inlineStr">
         <is>
-          <t>10:57:28</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>Russian Premier League</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="inlineStr">
-        <is>
-          <t>Rostov</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>Spartak Moscovo</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="inlineStr">
-        <is>
-          <t>25'</t>
-        </is>
-      </c>
-      <c r="G7" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="H7" s="2" t="inlineStr">
-        <is>
-          <t>Em Andamento</t>
-        </is>
-      </c>
-      <c r="I7" s="2" t="inlineStr">
-        <is>
-          <t>06/04/2025</t>
-        </is>
-      </c>
-      <c r="J7" s="2" t="inlineStr">
-        <is>
-          <t>10:57:29</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>Scottish Premiership</t>
-        </is>
-      </c>
-      <c r="B8" s="2" t="inlineStr">
-        <is>
-          <t>Heart of Midlothian FC</t>
-        </is>
-      </c>
-      <c r="C8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="inlineStr">
-        <is>
-          <t>Dundee United</t>
-        </is>
-      </c>
-      <c r="E8" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2" t="inlineStr">
-        <is>
-          <t>25'</t>
-        </is>
-      </c>
-      <c r="G8" s="2" t="n">
-        <v>25</v>
-      </c>
-      <c r="H8" s="2" t="inlineStr">
-        <is>
-          <t>Em Andamento</t>
-        </is>
-      </c>
-      <c r="I8" s="2" t="inlineStr">
-        <is>
-          <t>06/04/2025</t>
-        </is>
-      </c>
-      <c r="J8" s="2" t="inlineStr">
-        <is>
-          <t>10:57:30</t>
+          <t>11:42:34</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J8"/>
+  <autoFilter ref="A1:J6"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adiciona cálculo e exibição do horário da próxima execução no loop automático
</commit_message>
<xml_diff>
--- a/Relatorio_Jogos_0x0.xlsx
+++ b/Relatorio_Jogos_0x0.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Jogos 0x0" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Jogos 0x0'!$A$1:$J$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Jogos 0x0'!$A$1:$J$2</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -514,12 +514,12 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Campeonato Islandês</t>
+          <t>Süper Lig</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>Valur Reykjavik</t>
+          <t>Fenerbahce</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
@@ -527,7 +527,7 @@
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>IF Vestri</t>
+          <t>Trabzonspor</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
@@ -553,196 +553,12 @@
       </c>
       <c r="J2" s="2" t="inlineStr">
         <is>
-          <t>11:42:30</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Liga Nacional de Futebol</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Torpedo Moscovo</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>SK Rotor Volgograd</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="inlineStr">
-        <is>
-          <t>40'</t>
-        </is>
-      </c>
-      <c r="G3" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="H3" s="2" t="inlineStr">
-        <is>
-          <t>Em Andamento</t>
-        </is>
-      </c>
-      <c r="I3" s="2" t="inlineStr">
-        <is>
-          <t>06/04/2025</t>
-        </is>
-      </c>
-      <c r="J3" s="2" t="inlineStr">
-        <is>
-          <t>11:42:31</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Liga Principal</t>
-        </is>
-      </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>FC Gomel</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>FC Slavia Mozyr</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="inlineStr">
-        <is>
-          <t>40'</t>
-        </is>
-      </c>
-      <c r="G4" s="2" t="n">
-        <v>40</v>
-      </c>
-      <c r="H4" s="2" t="inlineStr">
-        <is>
-          <t>Em Andamento</t>
-        </is>
-      </c>
-      <c r="I4" s="2" t="inlineStr">
-        <is>
-          <t>06/04/2025</t>
-        </is>
-      </c>
-      <c r="J4" s="2" t="inlineStr">
-        <is>
-          <t>11:42:32</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Primeira Liga de Futebol Profissional</t>
-        </is>
-      </c>
-      <c r="B5" s="2" t="inlineStr">
-        <is>
-          <t>Beroe Stara Zagora</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>Levski Sófia</t>
-        </is>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>24'</t>
-        </is>
-      </c>
-      <c r="G5" s="2" t="n">
-        <v>24</v>
-      </c>
-      <c r="H5" s="2" t="inlineStr">
-        <is>
-          <t>Em Andamento</t>
-        </is>
-      </c>
-      <c r="I5" s="2" t="inlineStr">
-        <is>
-          <t>06/04/2025</t>
-        </is>
-      </c>
-      <c r="J5" s="2" t="inlineStr">
-        <is>
-          <t>11:42:33</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Torneo Federal A</t>
-        </is>
-      </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>CD Santamarina Tandil</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>Deportivo Rincón</t>
-        </is>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="inlineStr">
-        <is>
-          <t>36'</t>
-        </is>
-      </c>
-      <c r="G6" s="2" t="n">
-        <v>36</v>
-      </c>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>Em Andamento</t>
-        </is>
-      </c>
-      <c r="I6" s="2" t="inlineStr">
-        <is>
-          <t>06/04/2025</t>
-        </is>
-      </c>
-      <c r="J6" s="2" t="inlineStr">
-        <is>
-          <t>11:42:34</t>
+          <t>13:43:15</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J6"/>
+  <autoFilter ref="A1:J2"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>